<commit_message>
Update 20240521 - Cas Perigord.xlsx
</commit_message>
<xml_diff>
--- a/SES202/20240521 - Cas Perigord.xlsx
+++ b/SES202/20240521 - Cas Perigord.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexis Joulié\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaalokkang/Desktop/TelecomParis_Promo2025/SES202/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA42349-A3C5-4FFC-965E-87B292A3EE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A96D867-A996-EB4A-9F7D-443ADF0E404A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{C60EBFE3-1D85-4E63-9BCD-62E9B002E174}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{C60EBFE3-1D85-4E63-9BCD-62E9B002E174}"/>
   </bookViews>
   <sheets>
     <sheet name="Cas Perigord avant Invest" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Cas Perigord avant Invest'!$AN$37:$AQ$75</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Cas Perigord avant Invest'!$B:$B</definedName>
     <definedName name="Tag862028162">9752269</definedName>
     <definedName name="TVA" localSheetId="0">'Cas Perigord avant Invest'!#REF!</definedName>
     <definedName name="TVA">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Cas Perigord avant Invest'!$AN$37:$AQ$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,12 +31,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Table d'hypothèses :</t>
   </si>
@@ -182,28 +177,91 @@
   <si>
     <t>Résultat d'Exploitation</t>
   </si>
+  <si>
+    <t>Bilan</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Immobilisations brutes</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amortissements cumulés</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Immobilisations nettes</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>Dettes Fournisseurs</t>
+  </si>
+  <si>
+    <t>BFR / Besoin en Fonds de Roulement</t>
+  </si>
+  <si>
+    <t>Trésorerie Disponible</t>
+  </si>
+  <si>
+    <t>Dettes Financières</t>
+  </si>
+  <si>
+    <t>Trésorerie Nette / (Dette Nette)</t>
+  </si>
+  <si>
+    <t>Capital Social</t>
+  </si>
+  <si>
+    <t>Réserves et Résultats Cumulés</t>
+  </si>
+  <si>
+    <t>Capitaux Propres</t>
+  </si>
+  <si>
+    <t>Capital social</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dividendes</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flux de trésorerie de financement</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Net Cash Flow</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Créances Clients</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="#,##0_);\(#,##0\);\-_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\);\-_)"/>
-    <numFmt numFmtId="166" formatCode="[$-40C]mmm\-yy;@"/>
+    <numFmt numFmtId="176" formatCode="#,##0_);\(#,##0\);\-_)"/>
+    <numFmt numFmtId="177" formatCode="#,##0.0_);\(#,##0.0\);\-_)"/>
+    <numFmt numFmtId="178" formatCode="[$-40C]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -268,6 +326,19 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -314,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -323,27 +394,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -353,22 +424,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,9 +476,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -429,7 +516,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -535,7 +622,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -677,7 +764,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,33 +772,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC552F-F630-43FE-BB85-A32265F8A1CD}">
-  <dimension ref="B2:AQ68"/>
+  <dimension ref="B2:AQ93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScale="166" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.1328125" style="1" customWidth="1"/>
-    <col min="3" max="39" width="10.73046875" style="1"/>
-    <col min="40" max="40" width="2.73046875" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" style="1" customWidth="1"/>
+    <col min="3" max="39" width="10.6640625" style="1"/>
+    <col min="40" max="40" width="2.6640625" style="1" customWidth="1"/>
+    <col min="41" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:43" ht="15" customHeight="1">
       <c r="B2" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:43" ht="15" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:43" ht="15" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -722,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:43" ht="15" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -730,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:43" ht="15" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -738,7 +825,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:43" ht="15" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -746,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:43" ht="15" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -754,7 +841,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:43" ht="15" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
@@ -762,7 +849,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:43" ht="15" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
@@ -770,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:43" ht="15" customHeight="1">
       <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
@@ -920,7 +1007,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="14" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:43" ht="15" customHeight="1">
       <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
@@ -1070,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:43" ht="15" customHeight="1">
       <c r="B16" s="11" t="s">
         <v>6</v>
       </c>
@@ -1231,7 +1318,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="18" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:43" ht="15" customHeight="1">
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1392,10 +1479,10 @@
         <v>8010</v>
       </c>
     </row>
-    <row r="19" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:43" ht="15" customHeight="1">
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:43" ht="15" customHeight="1">
       <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1418,7 +1505,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:43" ht="15" customHeight="1">
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1444,7 +1531,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="22" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:43" ht="15" customHeight="1">
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1470,7 +1557,7 @@
         <v>45047</v>
       </c>
     </row>
-    <row r="23" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:43" ht="15" customHeight="1">
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1496,20 +1583,20 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="24" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:43" ht="15" customHeight="1">
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:43" ht="15" customHeight="1">
       <c r="B25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D25" s="4" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D26)</f>
-        <v>=SI(D$16=$G21;-$C21;0)</v>
+        <v>=IF(D$16=$G21;-$C21;0)</v>
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:43" ht="15" customHeight="1">
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1658,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:43" ht="15" customHeight="1">
       <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1807,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:43" ht="15" customHeight="1">
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1956,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:43" ht="15" customHeight="1">
       <c r="B29" s="2" t="s">
         <v>41</v>
       </c>
@@ -2105,20 +2192,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:43" ht="15" customHeight="1">
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:43" ht="15" customHeight="1">
       <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="4" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D32)</f>
-        <v>=SI(D$16&gt;=$G21;SI(D$16&lt;=$H21;-$F21;0);0)</v>
+        <v>=IF(D$16&gt;=$G21;IF(D$16&lt;=$H21;-$F21;0);0)</v>
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:43" ht="15" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2267,7 +2354,7 @@
         <v>-13.888888888888889</v>
       </c>
     </row>
-    <row r="33" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:43" ht="15" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>26</v>
       </c>
@@ -2416,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:43" ht="15" customHeight="1">
       <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
@@ -2565,7 +2652,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="35" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:43" ht="15" customHeight="1">
       <c r="B35" s="2" t="s">
         <v>41</v>
       </c>
@@ -2714,10 +2801,10 @@
         <v>-18.888888888888889</v>
       </c>
     </row>
-    <row r="36" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:43" ht="15" customHeight="1">
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:43" ht="15" customHeight="1">
       <c r="B37" s="11" t="s">
         <v>9</v>
       </c>
@@ -2879,7 +2966,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="39" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:43" ht="15" customHeight="1">
       <c r="B39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3040,7 +3127,7 @@
         <v>64080</v>
       </c>
     </row>
-    <row r="40" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:43" ht="15" customHeight="1">
       <c r="B40" s="1" t="s">
         <v>11</v>
       </c>
@@ -3201,7 +3288,7 @@
         <v>-40050</v>
       </c>
     </row>
-    <row r="41" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:43" ht="15" customHeight="1">
       <c r="B41" s="2" t="s">
         <v>12</v>
       </c>
@@ -3363,7 +3450,7 @@
         <v>24030</v>
       </c>
     </row>
-    <row r="43" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:43" ht="15" customHeight="1">
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
@@ -3524,7 +3611,7 @@
         <v>-8400</v>
       </c>
     </row>
-    <row r="45" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:43" ht="15" customHeight="1">
       <c r="B45" s="2" t="s">
         <v>14</v>
       </c>
@@ -3686,17 +3773,17 @@
         <v>15630</v>
       </c>
     </row>
-    <row r="46" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:43" ht="15" customHeight="1">
       <c r="B46" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:43" ht="15" customHeight="1">
       <c r="B47" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:43" ht="15" customHeight="1">
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
@@ -3845,7 +3932,7 @@
         <v>-18.888888888888889</v>
       </c>
     </row>
-    <row r="51" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:43" ht="15" customHeight="1">
       <c r="B51" s="2" t="s">
         <v>44</v>
       </c>
@@ -3994,17 +4081,17 @@
         <v>1630.1111111111111</v>
       </c>
     </row>
-    <row r="52" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:43" ht="15" customHeight="1">
       <c r="B52" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:43" ht="15" customHeight="1">
       <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:43" ht="15" customHeight="1">
       <c r="B55" s="11" t="s">
         <v>17</v>
       </c>
@@ -4166,7 +4253,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="57" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:43" ht="15" customHeight="1">
       <c r="B57" s="1" t="s">
         <v>18</v>
       </c>
@@ -4321,7 +4408,7 @@
         <v>60048</v>
       </c>
     </row>
-    <row r="58" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:43" ht="15" customHeight="1">
       <c r="B58" s="1" t="s">
         <v>19</v>
       </c>
@@ -4479,7 +4566,7 @@
         <v>-38790</v>
       </c>
     </row>
-    <row r="59" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:43" ht="15" customHeight="1">
       <c r="B59" s="1" t="s">
         <v>13</v>
       </c>
@@ -4640,7 +4727,7 @@
         <v>-8400</v>
       </c>
     </row>
-    <row r="61" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:43" ht="15" customHeight="1">
       <c r="B61" s="2" t="s">
         <v>20</v>
       </c>
@@ -4801,7 +4888,7 @@
         <v>12858</v>
       </c>
     </row>
-    <row r="63" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:43" ht="15" customHeight="1">
       <c r="B63" s="2" t="s">
         <v>21</v>
       </c>
@@ -4962,7 +5049,7 @@
         <v>-180</v>
       </c>
     </row>
-    <row r="65" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:43" ht="15" customHeight="1">
       <c r="B65" s="17" t="s">
         <v>22</v>
       </c>
@@ -5112,19 +5199,19 @@
         <v>1418</v>
       </c>
       <c r="AO65" s="19">
-        <f t="shared" ref="AO65:AQ65" si="27">SUM(AO61,AO63)</f>
+        <f>SUM(AO61,AO63)</f>
         <v>-6095</v>
       </c>
       <c r="AP65" s="19">
-        <f t="shared" si="27"/>
+        <f>SUM(AP61,AP63)</f>
         <v>3786</v>
       </c>
       <c r="AQ65" s="19">
-        <f t="shared" si="27"/>
+        <f>SUM(AQ61,AQ63)</f>
         <v>12678</v>
       </c>
     </row>
-    <row r="66" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="2:43" ht="15" customHeight="1">
       <c r="B66" s="17" t="s">
         <v>23</v>
       </c>
@@ -5138,155 +5225,155 @@
         <v>-2140</v>
       </c>
       <c r="F66" s="19">
-        <f t="shared" ref="F66:AQ66" si="28">E66+F65</f>
+        <f t="shared" ref="F66:AQ66" si="27">E66+F65</f>
         <v>-2801</v>
       </c>
       <c r="G66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-3399</v>
       </c>
       <c r="H66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-3934</v>
       </c>
       <c r="I66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-4586</v>
       </c>
       <c r="J66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-4995</v>
       </c>
       <c r="K66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-5341</v>
       </c>
       <c r="L66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-5624</v>
       </c>
       <c r="M66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-5844</v>
       </c>
       <c r="N66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-6001</v>
       </c>
       <c r="O66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-6095</v>
       </c>
       <c r="P66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-6126</v>
       </c>
       <c r="Q66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-6094</v>
       </c>
       <c r="R66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-5999</v>
       </c>
       <c r="S66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-5841</v>
       </c>
       <c r="T66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-5620</v>
       </c>
       <c r="U66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-5336</v>
       </c>
       <c r="V66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-4989</v>
       </c>
       <c r="W66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-4579</v>
       </c>
       <c r="X66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-4106</v>
       </c>
       <c r="Y66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-3570</v>
       </c>
       <c r="Z66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-2971</v>
       </c>
       <c r="AA66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-2309</v>
       </c>
       <c r="AB66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-1764</v>
       </c>
       <c r="AC66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-976</v>
       </c>
       <c r="AD66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-125</v>
       </c>
       <c r="AE66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>789</v>
       </c>
       <c r="AF66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>1766</v>
       </c>
       <c r="AG66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2806</v>
       </c>
       <c r="AH66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>3909</v>
       </c>
       <c r="AI66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5075</v>
       </c>
       <c r="AJ66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>6304</v>
       </c>
       <c r="AK66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>7596</v>
       </c>
       <c r="AL66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>8951</v>
       </c>
       <c r="AM66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>10369</v>
       </c>
       <c r="AO66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-6095</v>
       </c>
       <c r="AP66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>-2309</v>
       </c>
       <c r="AQ66" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>10369</v>
       </c>
     </row>
-    <row r="68" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="2:43" ht="15" customHeight="1">
       <c r="B68" s="4" t="s">
         <v>24</v>
       </c>
@@ -5295,7 +5382,2607 @@
         <v>-6126</v>
       </c>
     </row>
+    <row r="69" spans="2:43" ht="15" customHeight="1">
+      <c r="B69" s="4"/>
+      <c r="C69" s="20"/>
+    </row>
+    <row r="70" spans="2:43" ht="15" customHeight="1">
+      <c r="B70" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" s="20"/>
+      <c r="D70" s="39">
+        <f>C10</f>
+        <v>10000</v>
+      </c>
+      <c r="E70" s="39">
+        <f t="shared" ref="E70:AM70" si="28">D10</f>
+        <v>0</v>
+      </c>
+      <c r="F70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="G70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="J70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="L70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="O70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="P70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="S70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="T70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="U70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="V70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="W70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="X70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Y70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Z70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AA70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AB70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AC70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AD70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AE70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AF70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AG70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AH70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AI70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AJ70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AK70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AL70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AM70" s="39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:43" ht="15" customHeight="1">
+      <c r="B71" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="20"/>
+      <c r="D71" s="39">
+        <v>0</v>
+      </c>
+      <c r="E71" s="39">
+        <v>0</v>
+      </c>
+      <c r="F71" s="39">
+        <v>0</v>
+      </c>
+      <c r="G71" s="39">
+        <v>0</v>
+      </c>
+      <c r="H71" s="39">
+        <v>0</v>
+      </c>
+      <c r="I71" s="39">
+        <v>0</v>
+      </c>
+      <c r="J71" s="39">
+        <v>0</v>
+      </c>
+      <c r="K71" s="39">
+        <v>0</v>
+      </c>
+      <c r="L71" s="39">
+        <v>0</v>
+      </c>
+      <c r="M71" s="39">
+        <v>0</v>
+      </c>
+      <c r="N71" s="39">
+        <v>0</v>
+      </c>
+      <c r="O71" s="39">
+        <v>0</v>
+      </c>
+      <c r="P71" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="39">
+        <v>0</v>
+      </c>
+      <c r="R71" s="39">
+        <v>0</v>
+      </c>
+      <c r="S71" s="39">
+        <v>0</v>
+      </c>
+      <c r="T71" s="39">
+        <v>0</v>
+      </c>
+      <c r="U71" s="39">
+        <v>0</v>
+      </c>
+      <c r="V71" s="39">
+        <v>0</v>
+      </c>
+      <c r="W71" s="39">
+        <v>0</v>
+      </c>
+      <c r="X71" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y71" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AA71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AE71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AG71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AH71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AK71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AL71" s="39">
+        <v>0</v>
+      </c>
+      <c r="AM71" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:43" ht="15" customHeight="1">
+      <c r="B72" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" s="20"/>
+      <c r="D72" s="9">
+        <f>SUM(D70:D71)</f>
+        <v>10000</v>
+      </c>
+      <c r="E72" s="9">
+        <f t="shared" ref="E72:AM72" si="29">SUM(E70:E71)</f>
+        <v>0</v>
+      </c>
+      <c r="F72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="G72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="H72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="K72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="L72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="M72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="P72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="Q72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="R72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="S72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="T72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="U72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="V72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="W72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="X72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="Y72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="Z72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AA72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AB72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AC72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AD72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AE72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AF72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AG72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AH72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AI72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AJ72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AK72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AL72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AM72" s="9">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:43" ht="15" customHeight="1">
+      <c r="B73" s="33"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="9"/>
+    </row>
+    <row r="74" spans="2:43" ht="15" customHeight="1">
+      <c r="B74" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" s="20"/>
+      <c r="D74" s="9">
+        <f>D72+D65</f>
+        <v>8800</v>
+      </c>
+      <c r="E74" s="9">
+        <f t="shared" ref="E74:AM74" si="30">E72+E65</f>
+        <v>-940</v>
+      </c>
+      <c r="F74" s="9">
+        <f t="shared" si="30"/>
+        <v>-661</v>
+      </c>
+      <c r="G74" s="9">
+        <f t="shared" si="30"/>
+        <v>-598</v>
+      </c>
+      <c r="H74" s="9">
+        <f t="shared" si="30"/>
+        <v>-535</v>
+      </c>
+      <c r="I74" s="9">
+        <f t="shared" si="30"/>
+        <v>-652</v>
+      </c>
+      <c r="J74" s="9">
+        <f t="shared" si="30"/>
+        <v>-409</v>
+      </c>
+      <c r="K74" s="9">
+        <f t="shared" si="30"/>
+        <v>-346</v>
+      </c>
+      <c r="L74" s="9">
+        <f t="shared" si="30"/>
+        <v>-283</v>
+      </c>
+      <c r="M74" s="9">
+        <f t="shared" si="30"/>
+        <v>-220</v>
+      </c>
+      <c r="N74" s="9">
+        <f t="shared" si="30"/>
+        <v>-157</v>
+      </c>
+      <c r="O74" s="9">
+        <f t="shared" si="30"/>
+        <v>-94</v>
+      </c>
+      <c r="P74" s="9">
+        <f t="shared" si="30"/>
+        <v>-31</v>
+      </c>
+      <c r="Q74" s="9">
+        <f t="shared" si="30"/>
+        <v>32</v>
+      </c>
+      <c r="R74" s="9">
+        <f t="shared" si="30"/>
+        <v>95</v>
+      </c>
+      <c r="S74" s="9">
+        <f t="shared" si="30"/>
+        <v>158</v>
+      </c>
+      <c r="T74" s="9">
+        <f t="shared" si="30"/>
+        <v>221</v>
+      </c>
+      <c r="U74" s="9">
+        <f t="shared" si="30"/>
+        <v>284</v>
+      </c>
+      <c r="V74" s="9">
+        <f t="shared" si="30"/>
+        <v>347</v>
+      </c>
+      <c r="W74" s="9">
+        <f t="shared" si="30"/>
+        <v>410</v>
+      </c>
+      <c r="X74" s="9">
+        <f t="shared" si="30"/>
+        <v>473</v>
+      </c>
+      <c r="Y74" s="9">
+        <f t="shared" si="30"/>
+        <v>536</v>
+      </c>
+      <c r="Z74" s="9">
+        <f t="shared" si="30"/>
+        <v>599</v>
+      </c>
+      <c r="AA74" s="9">
+        <f t="shared" si="30"/>
+        <v>662</v>
+      </c>
+      <c r="AB74" s="9">
+        <f t="shared" si="30"/>
+        <v>545</v>
+      </c>
+      <c r="AC74" s="9">
+        <f t="shared" si="30"/>
+        <v>788</v>
+      </c>
+      <c r="AD74" s="9">
+        <f t="shared" si="30"/>
+        <v>851</v>
+      </c>
+      <c r="AE74" s="9">
+        <f t="shared" si="30"/>
+        <v>914</v>
+      </c>
+      <c r="AF74" s="9">
+        <f t="shared" si="30"/>
+        <v>977</v>
+      </c>
+      <c r="AG74" s="9">
+        <f t="shared" si="30"/>
+        <v>1040</v>
+      </c>
+      <c r="AH74" s="9">
+        <f t="shared" si="30"/>
+        <v>1103</v>
+      </c>
+      <c r="AI74" s="9">
+        <f t="shared" si="30"/>
+        <v>1166</v>
+      </c>
+      <c r="AJ74" s="9">
+        <f t="shared" si="30"/>
+        <v>1229</v>
+      </c>
+      <c r="AK74" s="9">
+        <f t="shared" si="30"/>
+        <v>1292</v>
+      </c>
+      <c r="AL74" s="9">
+        <f t="shared" si="30"/>
+        <v>1355</v>
+      </c>
+      <c r="AM74" s="9">
+        <f t="shared" si="30"/>
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="76" spans="2:43" ht="15" customHeight="1">
+      <c r="B76" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="13">
+        <f>D$16</f>
+        <v>44197</v>
+      </c>
+      <c r="E76" s="13">
+        <f t="shared" ref="E76:AM76" si="31">E$16</f>
+        <v>44228</v>
+      </c>
+      <c r="F76" s="13">
+        <f t="shared" si="31"/>
+        <v>44256</v>
+      </c>
+      <c r="G76" s="13">
+        <f t="shared" si="31"/>
+        <v>44287</v>
+      </c>
+      <c r="H76" s="13">
+        <f t="shared" si="31"/>
+        <v>44317</v>
+      </c>
+      <c r="I76" s="13">
+        <f t="shared" si="31"/>
+        <v>44348</v>
+      </c>
+      <c r="J76" s="13">
+        <f t="shared" si="31"/>
+        <v>44378</v>
+      </c>
+      <c r="K76" s="13">
+        <f t="shared" si="31"/>
+        <v>44409</v>
+      </c>
+      <c r="L76" s="13">
+        <f t="shared" si="31"/>
+        <v>44440</v>
+      </c>
+      <c r="M76" s="13">
+        <f t="shared" si="31"/>
+        <v>44470</v>
+      </c>
+      <c r="N76" s="13">
+        <f t="shared" si="31"/>
+        <v>44501</v>
+      </c>
+      <c r="O76" s="13">
+        <f t="shared" si="31"/>
+        <v>44531</v>
+      </c>
+      <c r="P76" s="13">
+        <f t="shared" si="31"/>
+        <v>44562</v>
+      </c>
+      <c r="Q76" s="13">
+        <f t="shared" si="31"/>
+        <v>44593</v>
+      </c>
+      <c r="R76" s="13">
+        <f t="shared" si="31"/>
+        <v>44621</v>
+      </c>
+      <c r="S76" s="13">
+        <f t="shared" si="31"/>
+        <v>44652</v>
+      </c>
+      <c r="T76" s="13">
+        <f t="shared" si="31"/>
+        <v>44682</v>
+      </c>
+      <c r="U76" s="13">
+        <f t="shared" si="31"/>
+        <v>44713</v>
+      </c>
+      <c r="V76" s="13">
+        <f t="shared" si="31"/>
+        <v>44743</v>
+      </c>
+      <c r="W76" s="13">
+        <f t="shared" si="31"/>
+        <v>44774</v>
+      </c>
+      <c r="X76" s="13">
+        <f t="shared" si="31"/>
+        <v>44805</v>
+      </c>
+      <c r="Y76" s="13">
+        <f t="shared" si="31"/>
+        <v>44835</v>
+      </c>
+      <c r="Z76" s="13">
+        <f t="shared" si="31"/>
+        <v>44866</v>
+      </c>
+      <c r="AA76" s="13">
+        <f t="shared" si="31"/>
+        <v>44896</v>
+      </c>
+      <c r="AB76" s="13">
+        <f t="shared" si="31"/>
+        <v>44927</v>
+      </c>
+      <c r="AC76" s="13">
+        <f t="shared" si="31"/>
+        <v>44958</v>
+      </c>
+      <c r="AD76" s="13">
+        <f t="shared" si="31"/>
+        <v>44986</v>
+      </c>
+      <c r="AE76" s="13">
+        <f t="shared" si="31"/>
+        <v>45017</v>
+      </c>
+      <c r="AF76" s="13">
+        <f t="shared" si="31"/>
+        <v>45047</v>
+      </c>
+      <c r="AG76" s="13">
+        <f t="shared" si="31"/>
+        <v>45078</v>
+      </c>
+      <c r="AH76" s="13">
+        <f t="shared" si="31"/>
+        <v>45108</v>
+      </c>
+      <c r="AI76" s="13">
+        <f t="shared" si="31"/>
+        <v>45139</v>
+      </c>
+      <c r="AJ76" s="13">
+        <f t="shared" si="31"/>
+        <v>45170</v>
+      </c>
+      <c r="AK76" s="13">
+        <f t="shared" si="31"/>
+        <v>45200</v>
+      </c>
+      <c r="AL76" s="13">
+        <f t="shared" si="31"/>
+        <v>45231</v>
+      </c>
+      <c r="AM76" s="13">
+        <f t="shared" si="31"/>
+        <v>45261</v>
+      </c>
+      <c r="AO76" s="11">
+        <f>AO$16</f>
+        <v>2021</v>
+      </c>
+      <c r="AP76" s="11">
+        <f>AP$16</f>
+        <v>2022</v>
+      </c>
+      <c r="AQ76" s="11">
+        <f>AQ$16</f>
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="77" spans="2:43" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="B77" s="35"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="37"/>
+      <c r="K77" s="37"/>
+      <c r="L77" s="37"/>
+      <c r="M77" s="37"/>
+      <c r="N77" s="37"/>
+      <c r="O77" s="37"/>
+      <c r="P77" s="37"/>
+      <c r="Q77" s="37"/>
+      <c r="R77" s="37"/>
+      <c r="S77" s="37"/>
+      <c r="T77" s="37"/>
+      <c r="U77" s="37"/>
+      <c r="V77" s="37"/>
+      <c r="W77" s="37"/>
+      <c r="X77" s="37"/>
+      <c r="Y77" s="37"/>
+      <c r="Z77" s="37"/>
+      <c r="AA77" s="37"/>
+      <c r="AB77" s="37"/>
+      <c r="AC77" s="37"/>
+      <c r="AD77" s="37"/>
+      <c r="AE77" s="37"/>
+      <c r="AF77" s="37"/>
+      <c r="AG77" s="37"/>
+      <c r="AH77" s="37"/>
+      <c r="AI77" s="37"/>
+      <c r="AJ77" s="37"/>
+      <c r="AK77" s="37"/>
+      <c r="AL77" s="37"/>
+      <c r="AM77" s="37"/>
+      <c r="AO77" s="35"/>
+      <c r="AP77" s="35"/>
+      <c r="AQ77" s="35"/>
+    </row>
+    <row r="78" spans="2:43" ht="15" customHeight="1">
+      <c r="B78" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" s="9">
+        <f>SUM($C$21:$C$23)</f>
+        <v>860</v>
+      </c>
+      <c r="E78" s="9">
+        <f t="shared" ref="E78:AM78" si="32">SUM($C$21:$C$23)</f>
+        <v>860</v>
+      </c>
+      <c r="F78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="G78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="H78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="I78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="J78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="K78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="L78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="M78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="N78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="O78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="P78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="Q78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="R78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="S78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="T78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="U78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="V78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="W78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="X78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="Y78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="Z78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AA78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AB78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AC78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AD78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AE78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AF78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AG78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AH78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AI78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AJ78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AK78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AL78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AM78" s="9">
+        <f t="shared" si="32"/>
+        <v>860</v>
+      </c>
+      <c r="AO78" s="9">
+        <f t="shared" ref="AO78:AQ80" si="33">SUMIFS($D78:$AM78,$D$13:$AM$13,AO$16)</f>
+        <v>10320</v>
+      </c>
+      <c r="AP78" s="9">
+        <f t="shared" si="33"/>
+        <v>10320</v>
+      </c>
+      <c r="AQ78" s="9">
+        <f t="shared" si="33"/>
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="79" spans="2:43" ht="15" customHeight="1">
+      <c r="B79" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="9">
+        <f>C79+D49</f>
+        <v>-13.888888888888889</v>
+      </c>
+      <c r="E79" s="9">
+        <f t="shared" ref="E79:AM79" si="34">D79+E49</f>
+        <v>-27.777777777777779</v>
+      </c>
+      <c r="F79" s="9">
+        <f t="shared" si="34"/>
+        <v>-41.666666666666671</v>
+      </c>
+      <c r="G79" s="9">
+        <f t="shared" si="34"/>
+        <v>-55.555555555555557</v>
+      </c>
+      <c r="H79" s="9">
+        <f t="shared" si="34"/>
+        <v>-69.444444444444443</v>
+      </c>
+      <c r="I79" s="9">
+        <f t="shared" si="34"/>
+        <v>-90.833333333333329</v>
+      </c>
+      <c r="J79" s="9">
+        <f t="shared" si="34"/>
+        <v>-112.22222222222221</v>
+      </c>
+      <c r="K79" s="9">
+        <f t="shared" si="34"/>
+        <v>-133.61111111111111</v>
+      </c>
+      <c r="L79" s="9">
+        <f t="shared" si="34"/>
+        <v>-155</v>
+      </c>
+      <c r="M79" s="9">
+        <f t="shared" si="34"/>
+        <v>-176.38888888888889</v>
+      </c>
+      <c r="N79" s="9">
+        <f t="shared" si="34"/>
+        <v>-197.77777777777777</v>
+      </c>
+      <c r="O79" s="9">
+        <f t="shared" si="34"/>
+        <v>-219.16666666666666</v>
+      </c>
+      <c r="P79" s="9">
+        <f t="shared" si="34"/>
+        <v>-240.55555555555554</v>
+      </c>
+      <c r="Q79" s="9">
+        <f t="shared" si="34"/>
+        <v>-261.94444444444446</v>
+      </c>
+      <c r="R79" s="9">
+        <f t="shared" si="34"/>
+        <v>-283.33333333333337</v>
+      </c>
+      <c r="S79" s="9">
+        <f t="shared" si="34"/>
+        <v>-304.72222222222229</v>
+      </c>
+      <c r="T79" s="9">
+        <f t="shared" si="34"/>
+        <v>-326.1111111111112</v>
+      </c>
+      <c r="U79" s="9">
+        <f t="shared" si="34"/>
+        <v>-347.50000000000011</v>
+      </c>
+      <c r="V79" s="9">
+        <f t="shared" si="34"/>
+        <v>-368.88888888888903</v>
+      </c>
+      <c r="W79" s="9">
+        <f t="shared" si="34"/>
+        <v>-390.27777777777794</v>
+      </c>
+      <c r="X79" s="9">
+        <f t="shared" si="34"/>
+        <v>-411.66666666666686</v>
+      </c>
+      <c r="Y79" s="9">
+        <f t="shared" si="34"/>
+        <v>-433.05555555555577</v>
+      </c>
+      <c r="Z79" s="9">
+        <f t="shared" si="34"/>
+        <v>-454.44444444444468</v>
+      </c>
+      <c r="AA79" s="9">
+        <f t="shared" si="34"/>
+        <v>-475.8333333333336</v>
+      </c>
+      <c r="AB79" s="9">
+        <f t="shared" si="34"/>
+        <v>-502.22222222222251</v>
+      </c>
+      <c r="AC79" s="9">
+        <f t="shared" si="34"/>
+        <v>-528.61111111111143</v>
+      </c>
+      <c r="AD79" s="9">
+        <f t="shared" si="34"/>
+        <v>-555.00000000000034</v>
+      </c>
+      <c r="AE79" s="9">
+        <f t="shared" si="34"/>
+        <v>-581.38888888888926</v>
+      </c>
+      <c r="AF79" s="9">
+        <f t="shared" si="34"/>
+        <v>-607.77777777777817</v>
+      </c>
+      <c r="AG79" s="9">
+        <f t="shared" si="34"/>
+        <v>-626.66666666666708</v>
+      </c>
+      <c r="AH79" s="9">
+        <f t="shared" si="34"/>
+        <v>-645.555555555556</v>
+      </c>
+      <c r="AI79" s="9">
+        <f t="shared" si="34"/>
+        <v>-664.44444444444491</v>
+      </c>
+      <c r="AJ79" s="9">
+        <f t="shared" si="34"/>
+        <v>-683.33333333333383</v>
+      </c>
+      <c r="AK79" s="9">
+        <f t="shared" si="34"/>
+        <v>-702.22222222222274</v>
+      </c>
+      <c r="AL79" s="9">
+        <f t="shared" si="34"/>
+        <v>-721.11111111111165</v>
+      </c>
+      <c r="AM79" s="9">
+        <f t="shared" si="34"/>
+        <v>-740.00000000000057</v>
+      </c>
+      <c r="AO79" s="9">
+        <f t="shared" si="33"/>
+        <v>-1293.3333333333335</v>
+      </c>
+      <c r="AP79" s="9">
+        <f t="shared" si="33"/>
+        <v>-4298.3333333333348</v>
+      </c>
+      <c r="AQ79" s="9">
+        <f t="shared" si="33"/>
+        <v>-7558.3333333333385</v>
+      </c>
+    </row>
+    <row r="80" spans="2:43" ht="15" customHeight="1">
+      <c r="B80" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" s="9">
+        <f>SUM(D78,D79)</f>
+        <v>846.11111111111109</v>
+      </c>
+      <c r="E80" s="9">
+        <f t="shared" ref="E80:AM80" si="35">SUM(E78,E79)</f>
+        <v>832.22222222222217</v>
+      </c>
+      <c r="F80" s="9">
+        <f t="shared" si="35"/>
+        <v>818.33333333333337</v>
+      </c>
+      <c r="G80" s="9">
+        <f t="shared" si="35"/>
+        <v>804.44444444444446</v>
+      </c>
+      <c r="H80" s="9">
+        <f t="shared" si="35"/>
+        <v>790.55555555555554</v>
+      </c>
+      <c r="I80" s="9">
+        <f t="shared" si="35"/>
+        <v>769.16666666666663</v>
+      </c>
+      <c r="J80" s="9">
+        <f t="shared" si="35"/>
+        <v>747.77777777777783</v>
+      </c>
+      <c r="K80" s="9">
+        <f t="shared" si="35"/>
+        <v>726.38888888888891</v>
+      </c>
+      <c r="L80" s="9">
+        <f t="shared" si="35"/>
+        <v>705</v>
+      </c>
+      <c r="M80" s="9">
+        <f t="shared" si="35"/>
+        <v>683.61111111111109</v>
+      </c>
+      <c r="N80" s="9">
+        <f t="shared" si="35"/>
+        <v>662.22222222222217</v>
+      </c>
+      <c r="O80" s="9">
+        <f t="shared" si="35"/>
+        <v>640.83333333333337</v>
+      </c>
+      <c r="P80" s="9">
+        <f t="shared" si="35"/>
+        <v>619.44444444444446</v>
+      </c>
+      <c r="Q80" s="9">
+        <f t="shared" si="35"/>
+        <v>598.05555555555554</v>
+      </c>
+      <c r="R80" s="9">
+        <f t="shared" si="35"/>
+        <v>576.66666666666663</v>
+      </c>
+      <c r="S80" s="9">
+        <f t="shared" si="35"/>
+        <v>555.27777777777771</v>
+      </c>
+      <c r="T80" s="9">
+        <f t="shared" si="35"/>
+        <v>533.8888888888888</v>
+      </c>
+      <c r="U80" s="9">
+        <f t="shared" si="35"/>
+        <v>512.49999999999989</v>
+      </c>
+      <c r="V80" s="9">
+        <f t="shared" si="35"/>
+        <v>491.11111111111097</v>
+      </c>
+      <c r="W80" s="9">
+        <f t="shared" si="35"/>
+        <v>469.72222222222206</v>
+      </c>
+      <c r="X80" s="9">
+        <f t="shared" si="35"/>
+        <v>448.33333333333314</v>
+      </c>
+      <c r="Y80" s="9">
+        <f t="shared" si="35"/>
+        <v>426.94444444444423</v>
+      </c>
+      <c r="Z80" s="9">
+        <f t="shared" si="35"/>
+        <v>405.55555555555532</v>
+      </c>
+      <c r="AA80" s="9">
+        <f t="shared" si="35"/>
+        <v>384.1666666666664</v>
+      </c>
+      <c r="AB80" s="9">
+        <f t="shared" si="35"/>
+        <v>357.77777777777749</v>
+      </c>
+      <c r="AC80" s="9">
+        <f t="shared" si="35"/>
+        <v>331.38888888888857</v>
+      </c>
+      <c r="AD80" s="9">
+        <f t="shared" si="35"/>
+        <v>304.99999999999966</v>
+      </c>
+      <c r="AE80" s="9">
+        <f t="shared" si="35"/>
+        <v>278.61111111111074</v>
+      </c>
+      <c r="AF80" s="9">
+        <f t="shared" si="35"/>
+        <v>252.22222222222183</v>
+      </c>
+      <c r="AG80" s="9">
+        <f t="shared" si="35"/>
+        <v>233.33333333333292</v>
+      </c>
+      <c r="AH80" s="9">
+        <f t="shared" si="35"/>
+        <v>214.444444444444</v>
+      </c>
+      <c r="AI80" s="9">
+        <f t="shared" si="35"/>
+        <v>195.55555555555509</v>
+      </c>
+      <c r="AJ80" s="9">
+        <f t="shared" si="35"/>
+        <v>176.66666666666617</v>
+      </c>
+      <c r="AK80" s="9">
+        <f t="shared" si="35"/>
+        <v>157.77777777777726</v>
+      </c>
+      <c r="AL80" s="9">
+        <f t="shared" si="35"/>
+        <v>138.88888888888835</v>
+      </c>
+      <c r="AM80" s="9">
+        <f t="shared" si="35"/>
+        <v>119.99999999999943</v>
+      </c>
+      <c r="AO80" s="9">
+        <f t="shared" si="33"/>
+        <v>9026.6666666666679</v>
+      </c>
+      <c r="AP80" s="9">
+        <f t="shared" si="33"/>
+        <v>6021.6666666666652</v>
+      </c>
+      <c r="AQ80" s="9">
+        <f t="shared" si="33"/>
+        <v>2761.6666666666615</v>
+      </c>
+    </row>
+    <row r="82" spans="2:39" ht="15" customHeight="1">
+      <c r="B82" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9">
+        <v>0</v>
+      </c>
+      <c r="I82" s="9">
+        <v>0</v>
+      </c>
+      <c r="J82" s="9">
+        <v>0</v>
+      </c>
+      <c r="K82" s="9">
+        <v>0</v>
+      </c>
+      <c r="L82" s="9">
+        <v>0</v>
+      </c>
+      <c r="M82" s="9">
+        <v>0</v>
+      </c>
+      <c r="N82" s="9">
+        <v>0</v>
+      </c>
+      <c r="O82" s="9">
+        <v>0</v>
+      </c>
+      <c r="P82" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="9">
+        <v>0</v>
+      </c>
+      <c r="R82" s="9">
+        <v>0</v>
+      </c>
+      <c r="S82" s="9">
+        <v>0</v>
+      </c>
+      <c r="T82" s="9">
+        <v>0</v>
+      </c>
+      <c r="U82" s="9">
+        <v>0</v>
+      </c>
+      <c r="V82" s="9">
+        <v>0</v>
+      </c>
+      <c r="W82" s="9">
+        <v>0</v>
+      </c>
+      <c r="X82" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM82" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:39" ht="15" customHeight="1">
+      <c r="B83" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D83" s="9">
+        <v>0</v>
+      </c>
+      <c r="E83" s="9">
+        <v>0</v>
+      </c>
+      <c r="F83" s="9">
+        <v>0</v>
+      </c>
+      <c r="G83" s="9">
+        <v>0</v>
+      </c>
+      <c r="H83" s="9">
+        <v>0</v>
+      </c>
+      <c r="I83" s="9">
+        <v>0</v>
+      </c>
+      <c r="J83" s="9">
+        <v>0</v>
+      </c>
+      <c r="K83" s="9">
+        <v>0</v>
+      </c>
+      <c r="L83" s="9">
+        <v>0</v>
+      </c>
+      <c r="M83" s="9">
+        <v>0</v>
+      </c>
+      <c r="N83" s="9">
+        <v>0</v>
+      </c>
+      <c r="O83" s="9">
+        <v>0</v>
+      </c>
+      <c r="P83" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="9">
+        <v>0</v>
+      </c>
+      <c r="R83" s="9">
+        <v>0</v>
+      </c>
+      <c r="S83" s="9">
+        <v>0</v>
+      </c>
+      <c r="T83" s="9">
+        <v>0</v>
+      </c>
+      <c r="U83" s="9">
+        <v>0</v>
+      </c>
+      <c r="V83" s="9">
+        <v>0</v>
+      </c>
+      <c r="W83" s="9">
+        <v>0</v>
+      </c>
+      <c r="X83" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y83" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM83" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:39" ht="15" customHeight="1">
+      <c r="B84" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D84" s="9">
+        <f>C84+D40-D58</f>
+        <v>-240</v>
+      </c>
+      <c r="E84" s="9">
+        <f t="shared" ref="E84:AM84" si="36">D84+E40-E58</f>
+        <v>-345</v>
+      </c>
+      <c r="F84" s="9">
+        <f t="shared" si="36"/>
+        <v>-450</v>
+      </c>
+      <c r="G84" s="9">
+        <f t="shared" si="36"/>
+        <v>-555</v>
+      </c>
+      <c r="H84" s="9">
+        <f t="shared" si="36"/>
+        <v>-660</v>
+      </c>
+      <c r="I84" s="9">
+        <f t="shared" si="36"/>
+        <v>-765</v>
+      </c>
+      <c r="J84" s="9">
+        <f t="shared" si="36"/>
+        <v>-870</v>
+      </c>
+      <c r="K84" s="9">
+        <f t="shared" si="36"/>
+        <v>-975</v>
+      </c>
+      <c r="L84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1080</v>
+      </c>
+      <c r="M84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1185</v>
+      </c>
+      <c r="N84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1290</v>
+      </c>
+      <c r="O84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1395</v>
+      </c>
+      <c r="P84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1500</v>
+      </c>
+      <c r="Q84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1605</v>
+      </c>
+      <c r="R84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1710</v>
+      </c>
+      <c r="S84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1815</v>
+      </c>
+      <c r="T84" s="9">
+        <f t="shared" si="36"/>
+        <v>-1920</v>
+      </c>
+      <c r="U84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2025</v>
+      </c>
+      <c r="V84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2130</v>
+      </c>
+      <c r="W84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2235</v>
+      </c>
+      <c r="X84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2340</v>
+      </c>
+      <c r="Y84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2445</v>
+      </c>
+      <c r="Z84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2550</v>
+      </c>
+      <c r="AA84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2655</v>
+      </c>
+      <c r="AB84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2760</v>
+      </c>
+      <c r="AC84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2865</v>
+      </c>
+      <c r="AD84" s="9">
+        <f t="shared" si="36"/>
+        <v>-2970</v>
+      </c>
+      <c r="AE84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3075</v>
+      </c>
+      <c r="AF84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3180</v>
+      </c>
+      <c r="AG84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3285</v>
+      </c>
+      <c r="AH84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3390</v>
+      </c>
+      <c r="AI84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3495</v>
+      </c>
+      <c r="AJ84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3600</v>
+      </c>
+      <c r="AK84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3705</v>
+      </c>
+      <c r="AL84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3810</v>
+      </c>
+      <c r="AM84" s="9">
+        <f t="shared" si="36"/>
+        <v>-3915</v>
+      </c>
+    </row>
+    <row r="85" spans="2:39" s="33" customFormat="1" ht="15" customHeight="1">
+      <c r="B85" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D85" s="34">
+        <f>SUM(D82:D84)</f>
+        <v>-240</v>
+      </c>
+      <c r="E85" s="34">
+        <f t="shared" ref="E85:AM85" si="37">SUM(E82:E84)</f>
+        <v>-345</v>
+      </c>
+      <c r="F85" s="34">
+        <f t="shared" si="37"/>
+        <v>-450</v>
+      </c>
+      <c r="G85" s="34">
+        <f t="shared" si="37"/>
+        <v>-555</v>
+      </c>
+      <c r="H85" s="34">
+        <f t="shared" si="37"/>
+        <v>-660</v>
+      </c>
+      <c r="I85" s="34">
+        <f t="shared" si="37"/>
+        <v>-765</v>
+      </c>
+      <c r="J85" s="34">
+        <f t="shared" si="37"/>
+        <v>-870</v>
+      </c>
+      <c r="K85" s="34">
+        <f t="shared" si="37"/>
+        <v>-975</v>
+      </c>
+      <c r="L85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1080</v>
+      </c>
+      <c r="M85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1185</v>
+      </c>
+      <c r="N85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1290</v>
+      </c>
+      <c r="O85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1395</v>
+      </c>
+      <c r="P85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1500</v>
+      </c>
+      <c r="Q85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1605</v>
+      </c>
+      <c r="R85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1710</v>
+      </c>
+      <c r="S85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1815</v>
+      </c>
+      <c r="T85" s="34">
+        <f t="shared" si="37"/>
+        <v>-1920</v>
+      </c>
+      <c r="U85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2025</v>
+      </c>
+      <c r="V85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2130</v>
+      </c>
+      <c r="W85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2235</v>
+      </c>
+      <c r="X85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2340</v>
+      </c>
+      <c r="Y85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2445</v>
+      </c>
+      <c r="Z85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2550</v>
+      </c>
+      <c r="AA85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2655</v>
+      </c>
+      <c r="AB85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2760</v>
+      </c>
+      <c r="AC85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2865</v>
+      </c>
+      <c r="AD85" s="34">
+        <f t="shared" si="37"/>
+        <v>-2970</v>
+      </c>
+      <c r="AE85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3075</v>
+      </c>
+      <c r="AF85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3180</v>
+      </c>
+      <c r="AG85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3285</v>
+      </c>
+      <c r="AH85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3390</v>
+      </c>
+      <c r="AI85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3495</v>
+      </c>
+      <c r="AJ85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3600</v>
+      </c>
+      <c r="AK85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3705</v>
+      </c>
+      <c r="AL85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3810</v>
+      </c>
+      <c r="AM85" s="34">
+        <f t="shared" si="37"/>
+        <v>-3915</v>
+      </c>
+    </row>
+    <row r="87" spans="2:39" ht="15" customHeight="1">
+      <c r="B87" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D87" s="9">
+        <f>D66</f>
+        <v>-1200</v>
+      </c>
+      <c r="E87" s="9">
+        <f t="shared" ref="E87:AM87" si="38">E66</f>
+        <v>-2140</v>
+      </c>
+      <c r="F87" s="9">
+        <f t="shared" si="38"/>
+        <v>-2801</v>
+      </c>
+      <c r="G87" s="9">
+        <f t="shared" si="38"/>
+        <v>-3399</v>
+      </c>
+      <c r="H87" s="9">
+        <f t="shared" si="38"/>
+        <v>-3934</v>
+      </c>
+      <c r="I87" s="9">
+        <f t="shared" si="38"/>
+        <v>-4586</v>
+      </c>
+      <c r="J87" s="9">
+        <f t="shared" si="38"/>
+        <v>-4995</v>
+      </c>
+      <c r="K87" s="9">
+        <f t="shared" si="38"/>
+        <v>-5341</v>
+      </c>
+      <c r="L87" s="9">
+        <f t="shared" si="38"/>
+        <v>-5624</v>
+      </c>
+      <c r="M87" s="9">
+        <f t="shared" si="38"/>
+        <v>-5844</v>
+      </c>
+      <c r="N87" s="9">
+        <f t="shared" si="38"/>
+        <v>-6001</v>
+      </c>
+      <c r="O87" s="9">
+        <f t="shared" si="38"/>
+        <v>-6095</v>
+      </c>
+      <c r="P87" s="9">
+        <f t="shared" si="38"/>
+        <v>-6126</v>
+      </c>
+      <c r="Q87" s="9">
+        <f t="shared" si="38"/>
+        <v>-6094</v>
+      </c>
+      <c r="R87" s="9">
+        <f t="shared" si="38"/>
+        <v>-5999</v>
+      </c>
+      <c r="S87" s="9">
+        <f t="shared" si="38"/>
+        <v>-5841</v>
+      </c>
+      <c r="T87" s="9">
+        <f t="shared" si="38"/>
+        <v>-5620</v>
+      </c>
+      <c r="U87" s="9">
+        <f t="shared" si="38"/>
+        <v>-5336</v>
+      </c>
+      <c r="V87" s="9">
+        <f t="shared" si="38"/>
+        <v>-4989</v>
+      </c>
+      <c r="W87" s="9">
+        <f t="shared" si="38"/>
+        <v>-4579</v>
+      </c>
+      <c r="X87" s="9">
+        <f t="shared" si="38"/>
+        <v>-4106</v>
+      </c>
+      <c r="Y87" s="9">
+        <f t="shared" si="38"/>
+        <v>-3570</v>
+      </c>
+      <c r="Z87" s="9">
+        <f t="shared" si="38"/>
+        <v>-2971</v>
+      </c>
+      <c r="AA87" s="9">
+        <f t="shared" si="38"/>
+        <v>-2309</v>
+      </c>
+      <c r="AB87" s="9">
+        <f t="shared" si="38"/>
+        <v>-1764</v>
+      </c>
+      <c r="AC87" s="9">
+        <f t="shared" si="38"/>
+        <v>-976</v>
+      </c>
+      <c r="AD87" s="9">
+        <f t="shared" si="38"/>
+        <v>-125</v>
+      </c>
+      <c r="AE87" s="9">
+        <f t="shared" si="38"/>
+        <v>789</v>
+      </c>
+      <c r="AF87" s="9">
+        <f t="shared" si="38"/>
+        <v>1766</v>
+      </c>
+      <c r="AG87" s="9">
+        <f t="shared" si="38"/>
+        <v>2806</v>
+      </c>
+      <c r="AH87" s="9">
+        <f t="shared" si="38"/>
+        <v>3909</v>
+      </c>
+      <c r="AI87" s="9">
+        <f t="shared" si="38"/>
+        <v>5075</v>
+      </c>
+      <c r="AJ87" s="9">
+        <f t="shared" si="38"/>
+        <v>6304</v>
+      </c>
+      <c r="AK87" s="9">
+        <f t="shared" si="38"/>
+        <v>7596</v>
+      </c>
+      <c r="AL87" s="9">
+        <f t="shared" si="38"/>
+        <v>8951</v>
+      </c>
+      <c r="AM87" s="9">
+        <f t="shared" si="38"/>
+        <v>10369</v>
+      </c>
+    </row>
+    <row r="88" spans="2:39" ht="15" customHeight="1">
+      <c r="B88" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D88" s="9">
+        <v>0</v>
+      </c>
+      <c r="E88" s="9">
+        <v>0</v>
+      </c>
+      <c r="F88" s="9">
+        <v>0</v>
+      </c>
+      <c r="G88" s="9">
+        <v>0</v>
+      </c>
+      <c r="H88" s="9">
+        <v>0</v>
+      </c>
+      <c r="I88" s="9">
+        <v>0</v>
+      </c>
+      <c r="J88" s="9">
+        <v>0</v>
+      </c>
+      <c r="K88" s="9">
+        <v>0</v>
+      </c>
+      <c r="L88" s="9">
+        <v>0</v>
+      </c>
+      <c r="M88" s="9">
+        <v>0</v>
+      </c>
+      <c r="N88" s="9">
+        <v>0</v>
+      </c>
+      <c r="O88" s="9">
+        <v>0</v>
+      </c>
+      <c r="P88" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q88" s="9">
+        <v>0</v>
+      </c>
+      <c r="R88" s="9">
+        <v>0</v>
+      </c>
+      <c r="S88" s="9">
+        <v>0</v>
+      </c>
+      <c r="T88" s="9">
+        <v>0</v>
+      </c>
+      <c r="U88" s="9">
+        <v>0</v>
+      </c>
+      <c r="V88" s="9">
+        <v>0</v>
+      </c>
+      <c r="W88" s="9">
+        <v>0</v>
+      </c>
+      <c r="X88" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y88" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL88" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM88" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:39" s="33" customFormat="1" ht="15" customHeight="1">
+      <c r="B89" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D89" s="34">
+        <f>SUM(D87:D88)</f>
+        <v>-1200</v>
+      </c>
+      <c r="E89" s="34">
+        <f t="shared" ref="E89:AM89" si="39">SUM(E87:E88)</f>
+        <v>-2140</v>
+      </c>
+      <c r="F89" s="34">
+        <f t="shared" si="39"/>
+        <v>-2801</v>
+      </c>
+      <c r="G89" s="34">
+        <f t="shared" si="39"/>
+        <v>-3399</v>
+      </c>
+      <c r="H89" s="34">
+        <f t="shared" si="39"/>
+        <v>-3934</v>
+      </c>
+      <c r="I89" s="34">
+        <f t="shared" si="39"/>
+        <v>-4586</v>
+      </c>
+      <c r="J89" s="34">
+        <f t="shared" si="39"/>
+        <v>-4995</v>
+      </c>
+      <c r="K89" s="34">
+        <f t="shared" si="39"/>
+        <v>-5341</v>
+      </c>
+      <c r="L89" s="34">
+        <f t="shared" si="39"/>
+        <v>-5624</v>
+      </c>
+      <c r="M89" s="34">
+        <f t="shared" si="39"/>
+        <v>-5844</v>
+      </c>
+      <c r="N89" s="34">
+        <f t="shared" si="39"/>
+        <v>-6001</v>
+      </c>
+      <c r="O89" s="34">
+        <f t="shared" si="39"/>
+        <v>-6095</v>
+      </c>
+      <c r="P89" s="34">
+        <f t="shared" si="39"/>
+        <v>-6126</v>
+      </c>
+      <c r="Q89" s="34">
+        <f t="shared" si="39"/>
+        <v>-6094</v>
+      </c>
+      <c r="R89" s="34">
+        <f t="shared" si="39"/>
+        <v>-5999</v>
+      </c>
+      <c r="S89" s="34">
+        <f t="shared" si="39"/>
+        <v>-5841</v>
+      </c>
+      <c r="T89" s="34">
+        <f t="shared" si="39"/>
+        <v>-5620</v>
+      </c>
+      <c r="U89" s="34">
+        <f t="shared" si="39"/>
+        <v>-5336</v>
+      </c>
+      <c r="V89" s="34">
+        <f t="shared" si="39"/>
+        <v>-4989</v>
+      </c>
+      <c r="W89" s="34">
+        <f t="shared" si="39"/>
+        <v>-4579</v>
+      </c>
+      <c r="X89" s="34">
+        <f t="shared" si="39"/>
+        <v>-4106</v>
+      </c>
+      <c r="Y89" s="34">
+        <f t="shared" si="39"/>
+        <v>-3570</v>
+      </c>
+      <c r="Z89" s="34">
+        <f t="shared" si="39"/>
+        <v>-2971</v>
+      </c>
+      <c r="AA89" s="34">
+        <f t="shared" si="39"/>
+        <v>-2309</v>
+      </c>
+      <c r="AB89" s="34">
+        <f t="shared" si="39"/>
+        <v>-1764</v>
+      </c>
+      <c r="AC89" s="34">
+        <f t="shared" si="39"/>
+        <v>-976</v>
+      </c>
+      <c r="AD89" s="34">
+        <f t="shared" si="39"/>
+        <v>-125</v>
+      </c>
+      <c r="AE89" s="34">
+        <f t="shared" si="39"/>
+        <v>789</v>
+      </c>
+      <c r="AF89" s="34">
+        <f t="shared" si="39"/>
+        <v>1766</v>
+      </c>
+      <c r="AG89" s="34">
+        <f t="shared" si="39"/>
+        <v>2806</v>
+      </c>
+      <c r="AH89" s="34">
+        <f t="shared" si="39"/>
+        <v>3909</v>
+      </c>
+      <c r="AI89" s="34">
+        <f t="shared" si="39"/>
+        <v>5075</v>
+      </c>
+      <c r="AJ89" s="34">
+        <f t="shared" si="39"/>
+        <v>6304</v>
+      </c>
+      <c r="AK89" s="34">
+        <f t="shared" si="39"/>
+        <v>7596</v>
+      </c>
+      <c r="AL89" s="34">
+        <f t="shared" si="39"/>
+        <v>8951</v>
+      </c>
+      <c r="AM89" s="34">
+        <f t="shared" si="39"/>
+        <v>10369</v>
+      </c>
+    </row>
+    <row r="91" spans="2:39" ht="15" customHeight="1">
+      <c r="B91" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D91" s="34">
+        <v>0</v>
+      </c>
+      <c r="E91" s="34">
+        <v>0</v>
+      </c>
+      <c r="F91" s="34">
+        <v>0</v>
+      </c>
+      <c r="G91" s="34">
+        <v>0</v>
+      </c>
+      <c r="H91" s="34">
+        <v>0</v>
+      </c>
+      <c r="I91" s="34">
+        <v>0</v>
+      </c>
+      <c r="J91" s="34">
+        <v>0</v>
+      </c>
+      <c r="K91" s="34">
+        <v>0</v>
+      </c>
+      <c r="L91" s="34">
+        <v>0</v>
+      </c>
+      <c r="M91" s="34">
+        <v>0</v>
+      </c>
+      <c r="N91" s="34">
+        <v>0</v>
+      </c>
+      <c r="O91" s="34">
+        <v>0</v>
+      </c>
+      <c r="P91" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q91" s="34">
+        <v>0</v>
+      </c>
+      <c r="R91" s="34">
+        <v>0</v>
+      </c>
+      <c r="S91" s="34">
+        <v>0</v>
+      </c>
+      <c r="T91" s="34">
+        <v>0</v>
+      </c>
+      <c r="U91" s="34">
+        <v>0</v>
+      </c>
+      <c r="V91" s="34">
+        <v>0</v>
+      </c>
+      <c r="W91" s="34">
+        <v>0</v>
+      </c>
+      <c r="X91" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y91" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AD91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AE91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AF91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AG91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AH91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AI91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AK91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AL91" s="34">
+        <v>0</v>
+      </c>
+      <c r="AM91" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:39" ht="15" customHeight="1">
+      <c r="B92" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D92" s="9">
+        <f>C92+D45</f>
+        <v>-556</v>
+      </c>
+      <c r="E92" s="9">
+        <f t="shared" ref="E92:AM92" si="40">D92+E45</f>
+        <v>-1049</v>
+      </c>
+      <c r="F92" s="9">
+        <f t="shared" si="40"/>
+        <v>-1479</v>
+      </c>
+      <c r="G92" s="9">
+        <f t="shared" si="40"/>
+        <v>-1846</v>
+      </c>
+      <c r="H92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2150</v>
+      </c>
+      <c r="I92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2391</v>
+      </c>
+      <c r="J92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2569</v>
+      </c>
+      <c r="K92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2684</v>
+      </c>
+      <c r="L92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2736</v>
+      </c>
+      <c r="M92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2725</v>
+      </c>
+      <c r="N92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2651</v>
+      </c>
+      <c r="O92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2514</v>
+      </c>
+      <c r="P92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2314</v>
+      </c>
+      <c r="Q92" s="9">
+        <f t="shared" si="40"/>
+        <v>-2051</v>
+      </c>
+      <c r="R92" s="9">
+        <f t="shared" si="40"/>
+        <v>-1725</v>
+      </c>
+      <c r="S92" s="9">
+        <f t="shared" si="40"/>
+        <v>-1336</v>
+      </c>
+      <c r="T92" s="9">
+        <f t="shared" si="40"/>
+        <v>-884</v>
+      </c>
+      <c r="U92" s="9">
+        <f t="shared" si="40"/>
+        <v>-369</v>
+      </c>
+      <c r="V92" s="9">
+        <f t="shared" si="40"/>
+        <v>209</v>
+      </c>
+      <c r="W92" s="9">
+        <f t="shared" si="40"/>
+        <v>850</v>
+      </c>
+      <c r="X92" s="9">
+        <f t="shared" si="40"/>
+        <v>1554</v>
+      </c>
+      <c r="Y92" s="9">
+        <f t="shared" si="40"/>
+        <v>2321</v>
+      </c>
+      <c r="Z92" s="9">
+        <f t="shared" si="40"/>
+        <v>3151</v>
+      </c>
+      <c r="AA92" s="9">
+        <f t="shared" si="40"/>
+        <v>4044</v>
+      </c>
+      <c r="AB92" s="9">
+        <f t="shared" si="40"/>
+        <v>5000</v>
+      </c>
+      <c r="AC92" s="9">
+        <f t="shared" si="40"/>
+        <v>6019</v>
+      </c>
+      <c r="AD92" s="9">
+        <f t="shared" si="40"/>
+        <v>7101</v>
+      </c>
+      <c r="AE92" s="9">
+        <f t="shared" si="40"/>
+        <v>8246</v>
+      </c>
+      <c r="AF92" s="9">
+        <f t="shared" si="40"/>
+        <v>9454</v>
+      </c>
+      <c r="AG92" s="9">
+        <f t="shared" si="40"/>
+        <v>10725</v>
+      </c>
+      <c r="AH92" s="9">
+        <f t="shared" si="40"/>
+        <v>12059</v>
+      </c>
+      <c r="AI92" s="9">
+        <f t="shared" si="40"/>
+        <v>13456</v>
+      </c>
+      <c r="AJ92" s="9">
+        <f t="shared" si="40"/>
+        <v>14916</v>
+      </c>
+      <c r="AK92" s="9">
+        <f t="shared" si="40"/>
+        <v>16439</v>
+      </c>
+      <c r="AL92" s="9">
+        <f t="shared" si="40"/>
+        <v>18025</v>
+      </c>
+      <c r="AM92" s="9">
+        <f t="shared" si="40"/>
+        <v>19674</v>
+      </c>
+    </row>
+    <row r="93" spans="2:39" ht="15" customHeight="1">
+      <c r="B93" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D93" s="9">
+        <f>SUM(D91:D92)</f>
+        <v>-556</v>
+      </c>
+      <c r="E93" s="9">
+        <f t="shared" ref="E93:AM93" si="41">SUM(E91:E92)</f>
+        <v>-1049</v>
+      </c>
+      <c r="F93" s="9">
+        <f t="shared" si="41"/>
+        <v>-1479</v>
+      </c>
+      <c r="G93" s="9">
+        <f t="shared" si="41"/>
+        <v>-1846</v>
+      </c>
+      <c r="H93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2150</v>
+      </c>
+      <c r="I93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2391</v>
+      </c>
+      <c r="J93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2569</v>
+      </c>
+      <c r="K93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2684</v>
+      </c>
+      <c r="L93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2736</v>
+      </c>
+      <c r="M93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2725</v>
+      </c>
+      <c r="N93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2651</v>
+      </c>
+      <c r="O93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2514</v>
+      </c>
+      <c r="P93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2314</v>
+      </c>
+      <c r="Q93" s="9">
+        <f t="shared" si="41"/>
+        <v>-2051</v>
+      </c>
+      <c r="R93" s="9">
+        <f t="shared" si="41"/>
+        <v>-1725</v>
+      </c>
+      <c r="S93" s="9">
+        <f t="shared" si="41"/>
+        <v>-1336</v>
+      </c>
+      <c r="T93" s="9">
+        <f t="shared" si="41"/>
+        <v>-884</v>
+      </c>
+      <c r="U93" s="9">
+        <f t="shared" si="41"/>
+        <v>-369</v>
+      </c>
+      <c r="V93" s="9">
+        <f t="shared" si="41"/>
+        <v>209</v>
+      </c>
+      <c r="W93" s="9">
+        <f t="shared" si="41"/>
+        <v>850</v>
+      </c>
+      <c r="X93" s="9">
+        <f t="shared" si="41"/>
+        <v>1554</v>
+      </c>
+      <c r="Y93" s="9">
+        <f t="shared" si="41"/>
+        <v>2321</v>
+      </c>
+      <c r="Z93" s="9">
+        <f t="shared" si="41"/>
+        <v>3151</v>
+      </c>
+      <c r="AA93" s="9">
+        <f t="shared" si="41"/>
+        <v>4044</v>
+      </c>
+      <c r="AB93" s="9">
+        <f t="shared" si="41"/>
+        <v>5000</v>
+      </c>
+      <c r="AC93" s="9">
+        <f t="shared" si="41"/>
+        <v>6019</v>
+      </c>
+      <c r="AD93" s="9">
+        <f t="shared" si="41"/>
+        <v>7101</v>
+      </c>
+      <c r="AE93" s="9">
+        <f t="shared" si="41"/>
+        <v>8246</v>
+      </c>
+      <c r="AF93" s="9">
+        <f t="shared" si="41"/>
+        <v>9454</v>
+      </c>
+      <c r="AG93" s="9">
+        <f t="shared" si="41"/>
+        <v>10725</v>
+      </c>
+      <c r="AH93" s="9">
+        <f t="shared" si="41"/>
+        <v>12059</v>
+      </c>
+      <c r="AI93" s="9">
+        <f t="shared" si="41"/>
+        <v>13456</v>
+      </c>
+      <c r="AJ93" s="9">
+        <f t="shared" si="41"/>
+        <v>14916</v>
+      </c>
+      <c r="AK93" s="9">
+        <f t="shared" si="41"/>
+        <v>16439</v>
+      </c>
+      <c r="AL93" s="9">
+        <f t="shared" si="41"/>
+        <v>18025</v>
+      </c>
+      <c r="AM93" s="9">
+        <f t="shared" si="41"/>
+        <v>19674</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>

</xml_diff>